<commit_message>
úlltimo cambio en planilla excel
</commit_message>
<xml_diff>
--- a/M1U2/Comandos Git.xlsx
+++ b/M1U2/Comandos Git.xlsx
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -731,7 +731,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="75" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>42</v>
       </c>

</xml_diff>